<commit_message>
MVC UPDATE SISWA DKV
</commit_message>
<xml_diff>
--- a/temp_doc/PERTA UJIAN FIX DKV.xlsx
+++ b/temp_doc/PERTA UJIAN FIX DKV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A97AD0-9366-E04D-AEF1-35A18E9268D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00A1052E-5568-7D4E-9460-7484CB8A6652}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16380" xr2:uid="{B0018247-3466-0142-A6A2-4C9F9839E079}"/>
   </bookViews>
@@ -830,7 +830,7 @@
   <dimension ref="A1:G46"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47:XFD90"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
MVC UPDATE FITUR DELETE
</commit_message>
<xml_diff>
--- a/temp_doc/PERTA UJIAN FIX DKV.xlsx
+++ b/temp_doc/PERTA UJIAN FIX DKV.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/XAMPP/xamppfiles/htdocs/cbt2.0admin/temp_doc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{002C867C-364A-3E4C-AFA7-D399B106EECF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F42C3D5-FE2D-7641-99C1-AA5F210ED82A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16400" xr2:uid="{B0018247-3466-0142-A6A2-4C9F9839E079}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16360" xr2:uid="{B0018247-3466-0142-A6A2-4C9F9839E079}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -134,9 +134,6 @@
     <t>Yusron Al Fawaz</t>
   </si>
   <si>
-    <t>TJKT</t>
-  </si>
-  <si>
     <t>User123</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Pass123*</t>
+  </si>
+  <si>
+    <t>IPA</t>
   </si>
 </sst>
 </file>
@@ -657,7 +657,7 @@
   <dimension ref="A1:G93"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="D16" sqref="D16:D26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -696,22 +696,22 @@
         <v>1001</v>
       </c>
       <c r="B2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>7</v>
       </c>
       <c r="D2" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
         <v>32</v>
       </c>
-      <c r="F2" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -719,22 +719,22 @@
         <v>1002</v>
       </c>
       <c r="B3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C3" s="6" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="G3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -742,22 +742,22 @@
         <v>1003</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="6" t="s">
         <v>9</v>
       </c>
       <c r="D4" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E4" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -765,22 +765,22 @@
         <v>1004</v>
       </c>
       <c r="B5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C5" s="6" t="s">
         <v>10</v>
       </c>
       <c r="D5" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G5" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -788,22 +788,22 @@
         <v>1005</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D6" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E6" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -811,22 +811,22 @@
         <v>1006</v>
       </c>
       <c r="B7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D7" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -834,22 +834,22 @@
         <v>1007</v>
       </c>
       <c r="B8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>13</v>
       </c>
       <c r="D8" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E8" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="G8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -857,22 +857,22 @@
         <v>1008</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D9" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E9" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -880,22 +880,22 @@
         <v>1009</v>
       </c>
       <c r="B10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D10" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -903,22 +903,22 @@
         <v>1010</v>
       </c>
       <c r="B11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C11" s="6" t="s">
         <v>16</v>
       </c>
       <c r="D11" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E11" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="G11" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -926,22 +926,22 @@
         <v>1011</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12" s="6" t="s">
         <v>17</v>
       </c>
       <c r="D12" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G12" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -949,22 +949,22 @@
         <v>1012</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C13" s="6" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E13" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="G13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -972,22 +972,22 @@
         <v>1013</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C14" s="6" t="s">
         <v>19</v>
       </c>
       <c r="D14" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E14" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -995,22 +995,22 @@
         <v>1014</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C15" s="6" t="s">
         <v>20</v>
       </c>
       <c r="D15" s="4">
-        <v>1041404</v>
+        <v>1027404</v>
       </c>
       <c r="E15" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1018,22 +1018,22 @@
         <v>1015</v>
       </c>
       <c r="B16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C16" s="6" t="s">
         <v>21</v>
       </c>
       <c r="D16" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="G16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1041,22 +1041,22 @@
         <v>1016</v>
       </c>
       <c r="B17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C17" s="6" t="s">
         <v>22</v>
       </c>
       <c r="D17" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F17" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="G17" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1064,22 +1064,22 @@
         <v>1017</v>
       </c>
       <c r="B18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="6" t="s">
         <v>23</v>
       </c>
       <c r="D18" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E18" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F18" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1087,22 +1087,22 @@
         <v>1018</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C19" s="6" t="s">
         <v>24</v>
       </c>
       <c r="D19" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E19" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="G19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1110,22 +1110,22 @@
         <v>1019</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" s="6" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G20" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1133,22 +1133,22 @@
         <v>1020</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C21" s="6" t="s">
         <v>26</v>
       </c>
       <c r="D21" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G21" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1156,22 +1156,22 @@
         <v>1021</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C22" s="6" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E22" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G22" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1179,22 +1179,22 @@
         <v>1022</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="6" t="s">
         <v>28</v>
       </c>
       <c r="D23" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E23" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G23" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1202,22 +1202,22 @@
         <v>1023</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C24" s="6" t="s">
         <v>29</v>
       </c>
       <c r="D24" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E24" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1225,22 +1225,22 @@
         <v>1024</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C25" s="6" t="s">
         <v>30</v>
       </c>
       <c r="D25" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E25" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="21" thickBot="1" x14ac:dyDescent="0.25">
@@ -1248,22 +1248,22 @@
         <v>1025</v>
       </c>
       <c r="B26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C26" s="6" t="s">
         <v>31</v>
       </c>
       <c r="D26" s="4">
-        <v>1041404</v>
+        <v>1028404</v>
       </c>
       <c r="E26" t="s">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="F26" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="20" x14ac:dyDescent="0.2">

</xml_diff>